<commit_message>
Modified processingfile2.qmd, processeddate2.rds, and eda2.qmd.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,37 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nstev.000\Documents\MSDA\24Sum_DA 6833\Repositories\austinthrash-P2-portfolio\starter-analysis-exercise\data\raw-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67353E12-BC0A-42C1-93B0-A496B13BE8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="Data" sheetId="2" r:id="rId5"/>
-    <sheet name="Codebook" sheetId="3" r:id="rId6"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Codebook" sheetId="3" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
-  <si>
-    <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
-  </si>
-  <si>
-    <t>Numbers Sheet Name</t>
-  </si>
-  <si>
-    <t>Numbers Table Name</t>
-  </si>
-  <si>
-    <t>Excel Worksheet Name</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Height</t>
   </si>
@@ -66,9 +56,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Codebook</t>
-  </si>
-  <si>
     <t>Variable Name</t>
   </si>
   <si>
@@ -91,72 +78,52 @@
   </si>
   <si>
     <t>M/F/O/NA</t>
+  </si>
+  <si>
+    <t>blood type</t>
+  </si>
+  <si>
+    <t>A+, A-, B+, B-, O+, O-, AB+, AB- or NA</t>
+  </si>
+  <si>
+    <t>Body mass index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF040C28"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -184,47 +151,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,26 +170,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff5e88b1"/>
-      <rgbColor rgb="ffeef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF5E88B1"/>
+      <rgbColor rgb="FFEEF3F4"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -454,7 +450,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -473,7 +469,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -503,7 +499,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -529,7 +525,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -555,7 +551,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -581,7 +577,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -607,7 +603,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -633,7 +629,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -659,7 +655,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -685,7 +681,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -711,7 +707,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -724,9 +720,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -743,7 +745,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -762,7 +764,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -788,7 +790,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -814,7 +816,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -840,7 +842,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -866,7 +868,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -892,7 +894,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -918,7 +920,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -944,7 +946,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -970,7 +972,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -996,7 +998,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1009,9 +1011,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1025,7 +1033,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1044,7 +1052,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1074,7 +1082,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1100,7 +1108,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1126,7 +1134,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1152,7 +1160,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1178,7 +1186,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1204,7 +1212,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1230,7 +1238,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1256,7 +1264,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1282,7 +1290,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1295,418 +1303,367 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="1" max="6" width="8.86328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="1" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+    </row>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="3">
+        <v>180</v>
+      </c>
+      <c r="B2" s="3">
+        <v>80</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="3">
+        <v>175</v>
+      </c>
+      <c r="B3" s="3">
+        <v>70</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A5" s="3">
+        <v>178</v>
+      </c>
+      <c r="B5" s="3">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="3">
+        <v>192</v>
+      </c>
+      <c r="B6" s="3">
+        <v>90</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A8" s="3">
+        <v>156</v>
+      </c>
+      <c r="B8" s="3">
+        <v>90</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A9" s="3">
+        <v>166</v>
+      </c>
+      <c r="B9" s="3">
+        <v>110</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" t="s" s="5">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D10" location="'Data'!R1C1" tooltip="" display="Data"/>
-    <hyperlink ref="D12" location="'Codebook'!R1C1" tooltip="" display="Codebook"/>
-  </hyperlinks>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="5" width="8.85156" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="7">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="3">
+        <v>155</v>
+      </c>
+      <c r="B10" s="3">
+        <v>54</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A11" s="3">
+        <v>145</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7000</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A12" s="3">
+        <v>165</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="8">
-        <v>180</v>
-      </c>
-      <c r="B2" s="8">
-        <v>80</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="8">
-        <v>175</v>
-      </c>
-      <c r="B3" s="8">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s" s="9">
-        <v>12</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="B4" s="8">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8">
-        <v>178</v>
-      </c>
-      <c r="B5" s="8">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="8">
-        <v>192</v>
-      </c>
-      <c r="B6" s="8">
-        <v>90</v>
-      </c>
-      <c r="C6" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A13" s="3">
+        <v>133</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A14" s="3">
+        <v>166</v>
+      </c>
+      <c r="B14" s="3">
         <v>55</v>
       </c>
-      <c r="C7" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="8">
-        <v>156</v>
-      </c>
-      <c r="B8" s="8">
-        <v>90</v>
-      </c>
-      <c r="C8" t="s" s="9">
-        <v>12</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="8">
-        <v>166</v>
-      </c>
-      <c r="B9" s="8">
-        <v>110</v>
-      </c>
-      <c r="C9" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="8">
-        <v>155</v>
-      </c>
-      <c r="B10" s="8">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="8">
-        <v>145</v>
-      </c>
-      <c r="B11" s="8">
-        <v>7000</v>
-      </c>
-      <c r="C11" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="8">
-        <v>165</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="8">
-        <v>133</v>
-      </c>
-      <c r="B13" s="8">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="8">
-        <v>166</v>
-      </c>
-      <c r="B14" s="8">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="8">
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A15" s="3">
         <v>154</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="3">
         <v>50</v>
       </c>
-      <c r="C15" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="14.3516" style="11" customWidth="1"/>
-    <col min="2" max="2" width="30.3516" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.8516" style="11" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="1" customWidth="1"/>
+    <col min="4" max="6" width="8.86328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s" s="7">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s" s="7">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="9">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>